<commit_message>
Finished inputting minimum fights into spreadsheet. Need to adjust loot drop for crafting
</commit_message>
<xml_diff>
--- a/Zones.xlsx
+++ b/Zones.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="2" activeTab="4" xr2:uid="{C17BEB8E-A02F-43D4-B32F-FEE2218EF49A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{C17BEB8E-A02F-43D4-B32F-FEE2218EF49A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="54">
   <si>
     <t>Enemy</t>
   </si>
@@ -108,9 +108,6 @@
     <t>Z4-Secret</t>
   </si>
   <si>
-    <t>Z4-1B Again</t>
-  </si>
-  <si>
     <t>Z4-2F</t>
   </si>
   <si>
@@ -142,6 +139,57 @@
   </si>
   <si>
     <t>Spirit Puppets 2</t>
+  </si>
+  <si>
+    <t>1B Count</t>
+  </si>
+  <si>
+    <t>1B Max Count</t>
+  </si>
+  <si>
+    <t>Death Knight</t>
+  </si>
+  <si>
+    <t>Skeleton Priest</t>
+  </si>
+  <si>
+    <t>Secret &amp;1B Again Max</t>
+  </si>
+  <si>
+    <t>BLW Spirit</t>
+  </si>
+  <si>
+    <t>BW Spirit</t>
+  </si>
+  <si>
+    <t>Acolyte</t>
+  </si>
+  <si>
+    <t>2F Count</t>
+  </si>
+  <si>
+    <t>Skeleton Guard</t>
+  </si>
+  <si>
+    <t>Death Lord</t>
+  </si>
+  <si>
+    <t>1B</t>
+  </si>
+  <si>
+    <t>Secret &amp; 1B</t>
+  </si>
+  <si>
+    <t>SEC</t>
+  </si>
+  <si>
+    <t>2F</t>
+  </si>
+  <si>
+    <t>Minimal Resources</t>
+  </si>
+  <si>
+    <t>Quantity</t>
   </si>
 </sst>
 </file>
@@ -184,7 +232,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="13">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -232,31 +286,79 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{412305C8-027E-4AF3-BBD8-744050003FC2}" name="Table12" displayName="Table12" ref="A2:J7" totalsRowShown="0">
-  <autoFilter ref="A2:J7" xr:uid="{3ECCC950-267B-4748-BB09-9744E60C6695}"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{412305C8-027E-4AF3-BBD8-744050003FC2}" name="Table12" displayName="Table12" ref="A2:I10" totalsRowShown="0">
+  <autoFilter ref="A2:I10" xr:uid="{3ECCC950-267B-4748-BB09-9744E60C6695}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{AF5A20F0-600B-4D71-A34A-9AB7E387BF40}" name="Resource"/>
-    <tableColumn id="2" xr3:uid="{986F8739-B172-4EA6-8D87-F07A422786CA}" name="Z1" dataDxfId="5">
+    <tableColumn id="2" xr3:uid="{986F8739-B172-4EA6-8D87-F07A422786CA}" name="Z1" dataDxfId="12">
       <calculatedColumnFormula>Table2[[#This Row],[Total]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E357D56D-F125-4E8C-BF05-AB64B17469E3}" name="Z2" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{E357D56D-F125-4E8C-BF05-AB64B17469E3}" name="Z2" dataDxfId="11">
       <calculatedColumnFormula>'Z2 Iston Forest'!B3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A1010162-7C76-4C3D-8390-FAB6B8614E3A}" name="Z3" dataDxfId="6">
+    <tableColumn id="4" xr3:uid="{A1010162-7C76-4C3D-8390-FAB6B8614E3A}" name="Z3" dataDxfId="10">
       <calculatedColumnFormula>Table2511[[#This Row],[Total]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{5177A577-72ED-4896-8A97-3108C68D0F64}" name="Z4-Ext"/>
-    <tableColumn id="6" xr3:uid="{0D3BE69F-B7C5-47F2-B1EB-77D1B0D8A367}" name="Z4-1F"/>
-    <tableColumn id="7" xr3:uid="{D9217075-B537-4493-8A29-FA7720684F50}" name="Z4-1B" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{F452E7C1-5E2F-4854-A946-FE7E08F9AB94}" name="Z4-Secret" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{7817B54C-9E67-49AE-9A1E-DAAE0D13C33C}" name="Z4-1B Again" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{E000E4DC-D273-421F-9323-D2FDD90ABBBA}" name="Z4-2F" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{5177A577-72ED-4896-8A97-3108C68D0F64}" name="Z4-Ext">
+      <calculatedColumnFormula>'Z4 Fort Reon'!B2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{0D3BE69F-B7C5-47F2-B1EB-77D1B0D8A367}" name="Z4-1F" dataDxfId="4">
+      <calculatedColumnFormula>'Z4 Fort Reon'!C2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{D9217075-B537-4493-8A29-FA7720684F50}" name="Z4-1B" dataDxfId="3">
+      <calculatedColumnFormula>'Z4 Fort Reon'!D2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{F452E7C1-5E2F-4854-A946-FE7E08F9AB94}" name="Z4-Secret" dataDxfId="2">
+      <calculatedColumnFormula>'Z4 Fort Reon'!E2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{E000E4DC-D273-421F-9323-D2FDD90ABBBA}" name="Z4-2F" dataDxfId="1">
+      <calculatedColumnFormula>'Z4 Fort Reon'!F2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{34C29402-8D23-42CA-B6E1-97C41F0502EE}" name="Table181217" displayName="Table181217" ref="A11:Q25" totalsRowShown="0">
+  <autoFilter ref="A11:Q25" xr:uid="{95675CB4-287A-47B5-B264-8C654A59D321}"/>
+  <tableColumns count="17">
+    <tableColumn id="1" xr3:uid="{9A4BF864-4ADE-4F19-85F5-3C619E4AC11C}" name="Enemy"/>
+    <tableColumn id="2" xr3:uid="{370AD5BA-3CF3-46BA-B3BA-14EA1553E2C2}" name="EXP"/>
+    <tableColumn id="3" xr3:uid="{9DEE1D84-099C-49BA-AB04-F28932B701BF}" name="Copper"/>
+    <tableColumn id="7" xr3:uid="{25CB3223-3347-46BB-9DDA-6DE9E4DDD256}" name="Iron"/>
+    <tableColumn id="8" xr3:uid="{2AAE1A52-8E13-4AD1-8060-CDF5F598B857}" name="Leather"/>
+    <tableColumn id="9" xr3:uid="{363326E8-0D6E-4BE2-A036-14180AC55490}" name="Potion"/>
+    <tableColumn id="10" xr3:uid="{1E193F14-AA3F-4931-83B7-A2556694FC1B}" name="Mana Potion"/>
+    <tableColumn id="11" xr3:uid="{80F2185B-A82A-4596-9DDA-FA315D1E5A99}" name="Restorative"/>
+    <tableColumn id="12" xr3:uid="{EED61496-9936-4CF8-B848-439D630221A7}" name="Ext Count"/>
+    <tableColumn id="13" xr3:uid="{8A9D3609-490E-4327-9BB3-BF787B369E43}" name="Ext Max Count"/>
+    <tableColumn id="14" xr3:uid="{1794E323-27D3-4968-B474-EFE0D71D3327}" name="1F Count"/>
+    <tableColumn id="15" xr3:uid="{005FB8E0-0612-4C57-8463-71BCD97ED937}" name="1F Max Count"/>
+    <tableColumn id="4" xr3:uid="{E2059782-2128-498D-9412-F37B0F4B859C}" name="1B Count"/>
+    <tableColumn id="5" xr3:uid="{95239946-6051-4C5F-A85C-6A2D4EC9B01F}" name="1B Max Count"/>
+    <tableColumn id="6" xr3:uid="{E7FB3FF7-786E-4CDC-8F6B-0504DB5B9B97}" name="SEC"/>
+    <tableColumn id="16" xr3:uid="{BB45DBBC-D13A-458A-9706-84874DB2BF8D}" name="Secret &amp;1B Again Max"/>
+    <tableColumn id="17" xr3:uid="{09028B2A-00A4-4B56-96BF-55F256973AB5}" name="2F Count"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DEF77B6A-602D-4661-B705-A2DD3F137F9D}" name="Table3" displayName="Table3" ref="A19:B24" totalsRowShown="0">
+  <autoFilter ref="A19:B24" xr:uid="{2B573164-2133-45D6-AB07-87BCE50B93A3}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{5AB58A83-81EB-40F1-8325-972669A97F75}" name="Minimal Resources"/>
+    <tableColumn id="2" xr3:uid="{33EB6522-2C5C-4F1A-B733-B7ACA0F56F61}" name="Quantity" dataDxfId="0">
+      <calculatedColumnFormula>SUM(B3:H3)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7D737765-78DC-43AC-B1E4-85A5502C5E22}" name="Table1" displayName="Table1" ref="E2:I4" totalsRowShown="0">
   <autoFilter ref="E2:I4" xr:uid="{018B0E7A-DC1E-420B-A461-4D0D2F78E5C7}"/>
   <tableColumns count="5">
@@ -270,25 +372,12 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{66A3D37B-2E8C-483B-88B0-FE0CC538C547}" name="Table2" displayName="Table2" ref="A2:B7" totalsRowShown="0">
-  <autoFilter ref="A2:B7" xr:uid="{3CEF8D17-E6EB-4472-B441-93EB2DBD7CFA}"/>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{66A3D37B-2E8C-483B-88B0-FE0CC538C547}" name="Table2" displayName="Table2" ref="A2:B11" totalsRowShown="0">
+  <autoFilter ref="A2:B11" xr:uid="{3CEF8D17-E6EB-4472-B441-93EB2DBD7CFA}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{535D5567-E2EE-4D3A-9FE0-241F15D71BE8}" name="Resource"/>
-    <tableColumn id="2" xr3:uid="{8F124801-4C0B-4A10-BAA7-787E077BD267}" name="Total" dataDxfId="10">
-      <calculatedColumnFormula>Table1[Copper]*Table1[Count]</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C730CBCD-351C-418C-9FEC-D2318A7D51F4}" name="Table25" displayName="Table25" ref="A2:B6" totalsRowShown="0">
-  <autoFilter ref="A2:B6" xr:uid="{2FAAC14E-A5D7-4A84-A3B6-B1EDAB821A70}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{D9B68D78-4275-4C3D-A286-2B6395C1F9D0}" name="Resource"/>
-    <tableColumn id="2" xr3:uid="{1C0B04D6-6189-4AEC-B3CA-ECC5BF85BA40}" name="Total" dataDxfId="9">
+    <tableColumn id="2" xr3:uid="{8F124801-4C0B-4A10-BAA7-787E077BD267}" name="Total" dataDxfId="9">
       <calculatedColumnFormula>Table1[Copper]*Table1[Count]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -297,6 +386,19 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C730CBCD-351C-418C-9FEC-D2318A7D51F4}" name="Table25" displayName="Table25" ref="A2:B6" totalsRowShown="0">
+  <autoFilter ref="A2:B6" xr:uid="{2FAAC14E-A5D7-4A84-A3B6-B1EDAB821A70}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{D9B68D78-4275-4C3D-A286-2B6395C1F9D0}" name="Resource"/>
+    <tableColumn id="2" xr3:uid="{1C0B04D6-6189-4AEC-B3CA-ECC5BF85BA40}" name="Total" dataDxfId="8">
+      <calculatedColumnFormula>Table1[Copper]*Table1[Count]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{98B5C48C-5901-4B65-8235-E711CD3DECBD}" name="Table18" displayName="Table18" ref="E2:K6" totalsRowShown="0">
   <autoFilter ref="E2:K6" xr:uid="{E17E5A1E-0F01-4775-9099-0B2C191D1813}"/>
   <tableColumns count="7">
@@ -312,12 +414,12 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{16C024D5-E74F-4F03-9A76-BBDA16E8E62F}" name="Table2511" displayName="Table2511" ref="A2:B7" totalsRowShown="0">
-  <autoFilter ref="A2:B7" xr:uid="{DBE2E078-72EF-4FC6-AEB9-48CE4800D1A5}"/>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{16C024D5-E74F-4F03-9A76-BBDA16E8E62F}" name="Table2511" displayName="Table2511" ref="A2:B10" totalsRowShown="0">
+  <autoFilter ref="A2:B10" xr:uid="{DBE2E078-72EF-4FC6-AEB9-48CE4800D1A5}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{428DD592-B766-47F7-B4C4-BACD21A509A6}" name="Resource"/>
-    <tableColumn id="2" xr3:uid="{873B423A-D2AC-45AD-9BC7-3BD4CAA98A19}" name="Total" dataDxfId="8">
+    <tableColumn id="2" xr3:uid="{873B423A-D2AC-45AD-9BC7-3BD4CAA98A19}" name="Total" dataDxfId="7">
       <calculatedColumnFormula>Table1[Copper]*Table1[Count]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -325,7 +427,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{EB37C4BE-A12C-4E20-A031-400E09BE52AB}" name="Table1812" displayName="Table1812" ref="E2:L8" totalsRowShown="0">
   <autoFilter ref="E2:L8" xr:uid="{CD685764-4F94-45C3-8834-A95E979FC15A}"/>
   <tableColumns count="8">
@@ -342,36 +444,20 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{BEBA8B15-BA39-426D-AF3D-61CD9F7C163D}" name="Table251116" displayName="Table251116" ref="A2:C9" totalsRowShown="0">
-  <autoFilter ref="A2:C9" xr:uid="{C57296E8-F403-4B55-A10F-DC29DF91EC81}"/>
-  <tableColumns count="3">
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{BEBA8B15-BA39-426D-AF3D-61CD9F7C163D}" name="Table251116" displayName="Table251116" ref="A1:F8" totalsRowShown="0">
+  <autoFilter ref="A1:F8" xr:uid="{C57296E8-F403-4B55-A10F-DC29DF91EC81}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{E8BB58F5-2E7B-419C-AD08-15424C65D752}" name="Resource"/>
-    <tableColumn id="2" xr3:uid="{DE3CE257-1A5C-4195-9A67-4151184B2BC8}" name="Exterior" dataDxfId="0">
+    <tableColumn id="2" xr3:uid="{DE3CE257-1A5C-4195-9A67-4151184B2BC8}" name="Exterior" dataDxfId="6">
       <calculatedColumnFormula>SUMPRODUCT(Table181217[EXP], Table181217[Ext Count])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{962DEA61-692E-4CCA-A4FE-15816216BDE7}" name="1F"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{34C29402-8D23-42CA-B6E1-97C41F0502EE}" name="Table181217" displayName="Table181217" ref="A11:L17" totalsRowShown="0">
-  <autoFilter ref="A11:L17" xr:uid="{95675CB4-287A-47B5-B264-8C654A59D321}"/>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{9A4BF864-4ADE-4F19-85F5-3C619E4AC11C}" name="Enemy"/>
-    <tableColumn id="2" xr3:uid="{370AD5BA-3CF3-46BA-B3BA-14EA1553E2C2}" name="EXP"/>
-    <tableColumn id="3" xr3:uid="{9DEE1D84-099C-49BA-AB04-F28932B701BF}" name="Copper"/>
-    <tableColumn id="7" xr3:uid="{25CB3223-3347-46BB-9DDA-6DE9E4DDD256}" name="Iron"/>
-    <tableColumn id="8" xr3:uid="{2AAE1A52-8E13-4AD1-8060-CDF5F598B857}" name="Leather"/>
-    <tableColumn id="9" xr3:uid="{363326E8-0D6E-4BE2-A036-14180AC55490}" name="Potion"/>
-    <tableColumn id="10" xr3:uid="{1E193F14-AA3F-4931-83B7-A2556694FC1B}" name="Mana Potion"/>
-    <tableColumn id="11" xr3:uid="{80F2185B-A82A-4596-9DDA-FA315D1E5A99}" name="Restorative"/>
-    <tableColumn id="12" xr3:uid="{EED61496-9936-4CF8-B848-439D630221A7}" name="Ext Count"/>
-    <tableColumn id="13" xr3:uid="{8A9D3609-490E-4327-9BB3-BF787B369E43}" name="Ext Max Count"/>
-    <tableColumn id="14" xr3:uid="{1794E323-27D3-4968-B474-EFE0D71D3327}" name="1F Count"/>
-    <tableColumn id="15" xr3:uid="{005FB8E0-0612-4C57-8463-71BCD97ED937}" name="1F Max Count"/>
+    <tableColumn id="3" xr3:uid="{962DEA61-692E-4CCA-A4FE-15816216BDE7}" name="1F" dataDxfId="5">
+      <calculatedColumnFormula>SUMPRODUCT(Table181217[Copper], Table181217[1F Count])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{DFA865C7-94B2-4590-95FF-7904BB224151}" name="1B"/>
+    <tableColumn id="5" xr3:uid="{D84E43C0-80E3-446A-9DE4-2D3F6494F408}" name="Secret &amp; 1B"/>
+    <tableColumn id="6" xr3:uid="{2BD21B0C-3C2F-4031-92FD-966DE026B662}" name="2F"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -674,15 +760,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CDC0E5D-F65A-4CA7-9147-6EE9F3B768D7}">
-  <dimension ref="A2:J7"/>
+  <dimension ref="A2:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -710,11 +799,8 @@
       <c r="I2" t="s">
         <v>26</v>
       </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -730,12 +816,28 @@
         <f>Table2511[[#This Row],[Total]]</f>
         <v>2790</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <f>'Z4 Fort Reon'!B2</f>
+        <v>1970</v>
+      </c>
+      <c r="F3">
+        <f>'Z4 Fort Reon'!C2</f>
+        <v>1690</v>
+      </c>
+      <c r="G3" s="1">
+        <f>'Z4 Fort Reon'!D2</f>
+        <v>6120</v>
+      </c>
+      <c r="H3" s="1">
+        <f>'Z4 Fort Reon'!E2</f>
+        <v>6250</v>
+      </c>
+      <c r="I3" s="1">
+        <f>'Z4 Fort Reon'!F2</f>
+        <v>3660</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -751,12 +853,28 @@
         <f>Table2511[[#This Row],[Total]]</f>
         <v>565</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <f>'Z4 Fort Reon'!B3</f>
+        <v>405</v>
+      </c>
+      <c r="F4">
+        <f>'Z4 Fort Reon'!C3</f>
+        <v>350</v>
+      </c>
+      <c r="G4" s="1">
+        <f>'Z4 Fort Reon'!D3</f>
+        <v>1305</v>
+      </c>
+      <c r="H4" s="1">
+        <f>'Z4 Fort Reon'!E3</f>
+        <v>990</v>
+      </c>
+      <c r="I4" s="1">
+        <f>'Z4 Fort Reon'!F3</f>
+        <v>885</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -772,12 +890,28 @@
         <f>Table2511[[#This Row],[Total]]</f>
         <v>7.5000000000000009</v>
       </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <f>'Z4 Fort Reon'!B4</f>
+        <v>6.3000000000000007</v>
+      </c>
+      <c r="F5">
+        <f>'Z4 Fort Reon'!C4</f>
+        <v>5.1000000000000005</v>
+      </c>
+      <c r="G5" s="1">
+        <f>'Z4 Fort Reon'!D4</f>
+        <v>15.200000000000001</v>
+      </c>
+      <c r="H5" s="1">
+        <f>'Z4 Fort Reon'!E4</f>
+        <v>11.4</v>
+      </c>
+      <c r="I5" s="1">
+        <f>'Z4 Fort Reon'!F4</f>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -793,12 +927,28 @@
         <f>Table2511[[#This Row],[Total]]</f>
         <v>6.5</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <f>'Z4 Fort Reon'!B5</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F6">
+        <f>'Z4 Fort Reon'!C5</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G6" s="1">
+        <f>'Z4 Fort Reon'!D5</f>
+        <v>14.5</v>
+      </c>
+      <c r="H6" s="1">
+        <f>'Z4 Fort Reon'!E5</f>
+        <v>4</v>
+      </c>
+      <c r="I6" s="1">
+        <f>'Z4 Fort Reon'!F5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -814,25 +964,203 @@
         <f>Table2511[[#This Row],[Total]]</f>
         <v>1</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="E7">
+        <f>'Z4 Fort Reon'!B6</f>
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <f>'Z4 Fort Reon'!C6</f>
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <f>'Z4 Fort Reon'!D6</f>
+        <v>2</v>
+      </c>
+      <c r="H7" s="1">
+        <f>'Z4 Fort Reon'!E6</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <f>'Z4 Fort Reon'!F6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="1">
+        <f>Table2[[#This Row],[Total]]</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <f>'Z2 Iston Forest'!B8</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <f>Table2511[[#This Row],[Total]]</f>
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f>'Z4 Fort Reon'!B7</f>
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <f>'Z4 Fort Reon'!C7</f>
+        <v>1.2</v>
+      </c>
+      <c r="G8" s="1">
+        <f>'Z4 Fort Reon'!D7</f>
+        <v>2.7</v>
+      </c>
+      <c r="H8" s="1">
+        <f>'Z4 Fort Reon'!E7</f>
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <f>'Z4 Fort Reon'!F7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1">
+        <f>Table2[[#This Row],[Total]]</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <f>'Z2 Iston Forest'!B9</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <f>Table2511[[#This Row],[Total]]</f>
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f>'Z4 Fort Reon'!B8</f>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f>'Z4 Fort Reon'!C8</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <f>'Z4 Fort Reon'!D8</f>
+        <v>1</v>
+      </c>
+      <c r="H9" s="1">
+        <f>'Z4 Fort Reon'!E8</f>
+        <v>2.1</v>
+      </c>
+      <c r="I9" s="1">
+        <f>'Z4 Fort Reon'!F8</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <f>Table2[[#This Row],[Total]]</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <f>'Z2 Iston Forest'!B10</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <f>Table2511[[#This Row],[Total]]</f>
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f>'Z4 Fort Reon'!B9</f>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f>'Z4 Fort Reon'!C9</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <f>'Z4 Fort Reon'!D9</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <f>'Z4 Fort Reon'!E9</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <f>'Z4 Fort Reon'!F9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <f t="shared" ref="B20:B24" si="0">SUM(B3:H3)</f>
+        <v>22530</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <f>SUM(B4:H4)</f>
+        <v>3855</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>47.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>39.299999999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11C72B31-51A4-47A0-AF3B-C313CA41D09A}">
-  <dimension ref="A2:I7"/>
+  <dimension ref="A2:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,6 +1251,26 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1092,10 +1440,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01DAB6FD-0716-4C98-B563-70054503DF68}">
-  <dimension ref="A2:L8"/>
+  <dimension ref="A2:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:L8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,6 +1655,9 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
       <c r="E8" t="s">
         <v>18</v>
       </c>
@@ -1331,6 +1682,16 @@
         <v>0.2</v>
       </c>
       <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1345,89 +1706,210 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7539993-12A1-4A4C-A6C1-860EE11BEC95}">
-  <dimension ref="A2:L17"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H2" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <f>SUMPRODUCT(Table181217[EXP], Table181217[Ext Count])</f>
         <v>1970</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C2">
+        <f>SUMPRODUCT(Table181217[EXP], Table181217[1F Count])</f>
+        <v>1690</v>
+      </c>
+      <c r="D2">
+        <f>SUMPRODUCT(Table181217[EXP], Table181217[1B Count])</f>
+        <v>6120</v>
+      </c>
+      <c r="E2">
+        <f>SUMPRODUCT(Table181217[EXP], Table181217[SEC])</f>
+        <v>6250</v>
+      </c>
+      <c r="F2">
+        <f>SUMPRODUCT(Table181217[EXP], Table181217[2F Count])</f>
+        <v>3660</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="B3">
         <f>SUMPRODUCT(Table181217[Copper], Table181217[Ext Count])</f>
         <v>405</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C3">
+        <f>SUMPRODUCT(Table181217[Copper], Table181217[1F Count])</f>
+        <v>350</v>
+      </c>
+      <c r="D3">
+        <f>SUMPRODUCT(Table181217[Copper], Table181217[1B Count])</f>
+        <v>1305</v>
+      </c>
+      <c r="E3">
+        <f>SUMPRODUCT(Table181217[Copper], Table181217[SEC])</f>
+        <v>990</v>
+      </c>
+      <c r="F3">
+        <f>SUMPRODUCT(Table181217[Copper], Table181217[2F Count])</f>
+        <v>885</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
+      <c r="B4">
         <f>SUMPRODUCT(Table181217[Iron], Table181217[Ext Count])</f>
         <v>6.3000000000000007</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C4">
+        <f>SUMPRODUCT(Table181217[Iron], Table181217[1F Count])</f>
+        <v>5.1000000000000005</v>
+      </c>
+      <c r="D4">
+        <f>SUMPRODUCT(Table181217[Iron], Table181217[1B Count])</f>
+        <v>15.200000000000001</v>
+      </c>
+      <c r="E4">
+        <f>SUMPRODUCT(Table181217[Iron], Table181217[SEC])</f>
+        <v>11.4</v>
+      </c>
+      <c r="F4">
+        <f>SUMPRODUCT(Table181217[Iron], Table181217[2F Count])</f>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B5" s="1">
         <f>SUMPRODUCT(Table181217[Leather], Table181217[Ext Count])</f>
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <f>SUMPRODUCT(Table181217[Leather], Table181217[1F Count])</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D5">
+        <f>SUMPRODUCT(Table181217[Leather], Table181217[1B Count])</f>
+        <v>14.5</v>
+      </c>
+      <c r="E5">
+        <f>SUMPRODUCT(Table181217[Leather], Table181217[SEC])</f>
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <f>SUMPRODUCT(Table181217[Leather], Table181217[2F Count])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1">
+        <f>SUMPRODUCT(Table181217[Potion], Table181217[Ext Count])</f>
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <f>SUMPRODUCT(Table181217[Potion], Table181217[1F Count])</f>
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <f>SUMPRODUCT(Table181217[Potion], Table181217[1B Count])</f>
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <f>SUMPRODUCT(Table181217[Potion], Table181217[SEC])</f>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f>SUMPRODUCT(Table181217[Potion], Table181217[2F Count])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1">
-        <f>SUMPRODUCT(Table181217[Potion], Table181217[Ext Count])</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <f>SUMPRODUCT(Table181217[Mana Potion], Table181217[Ext Count])</f>
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <f>SUMPRODUCT(Table181217[Mana Potion], Table181217[1F Count])</f>
+        <v>1.2</v>
+      </c>
+      <c r="D7">
+        <f>SUMPRODUCT(Table181217[Mana Potion], Table181217[1B Count])</f>
+        <v>2.7</v>
+      </c>
+      <c r="E7">
+        <f>SUMPRODUCT(Table181217[Mana Potion], Table181217[SEC])</f>
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <f>SUMPRODUCT(Table181217[Mana Potion], Table181217[2F Count])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
       <c r="B8" s="1">
-        <f>SUMPRODUCT(Table181217[Mana Potion], Table181217[Ext Count])</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="1">
         <f>SUMPRODUCT(Table181217[Restorative], Table181217[Ext Count])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <f>SUMPRODUCT(Table181217[Restorative], Table181217[1F Count])</f>
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f>SUMPRODUCT(Table181217[Restorative], Table181217[1B Count])</f>
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <f>SUMPRODUCT(Table181217[Restorative], Table181217[SEC])</f>
+        <v>2.1</v>
+      </c>
+      <c r="F8">
+        <f>SUMPRODUCT(Table181217[Restorative], Table181217[2F Count])</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1447,25 +1929,40 @@
         <v>17</v>
       </c>
       <c r="G11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" t="s">
         <v>29</v>
       </c>
-      <c r="H11" t="s">
-        <v>30</v>
-      </c>
       <c r="I11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" t="s">
         <v>33</v>
       </c>
-      <c r="J11" t="s">
-        <v>36</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>34</v>
       </c>
-      <c r="L11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" t="s">
+        <v>37</v>
+      </c>
+      <c r="N11" t="s">
+        <v>38</v>
+      </c>
+      <c r="O11" t="s">
+        <v>50</v>
+      </c>
+      <c r="P11" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1501,8 +1998,14 @@
       <c r="K12">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <v>8</v>
+      </c>
+      <c r="O12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1537,8 +2040,14 @@
       <c r="K13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <v>4</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1574,8 +2083,17 @@
       <c r="K14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <v>9</v>
+      </c>
+      <c r="M14">
+        <v>22</v>
+      </c>
+      <c r="O14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1610,10 +2128,16 @@
       <c r="K15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <v>2</v>
+      </c>
+      <c r="M15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16">
         <v>180</v>
@@ -1645,10 +2169,16 @@
       <c r="K16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <v>2</v>
+      </c>
+      <c r="M16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17">
         <v>120</v>
@@ -1678,6 +2208,173 @@
       </c>
       <c r="K17">
         <v>2</v>
+      </c>
+      <c r="M17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18">
+        <v>1000</v>
+      </c>
+      <c r="C18">
+        <v>250</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19">
+        <v>180</v>
+      </c>
+      <c r="C19">
+        <v>35</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <f>1/2 + 0</f>
+        <v>0.5</v>
+      </c>
+      <c r="M19">
+        <v>2</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20">
+        <v>150</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <f>1/10 + 0</f>
+        <v>0.1</v>
+      </c>
+      <c r="O20">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21">
+        <v>500</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22">
+        <v>300</v>
+      </c>
+      <c r="C22">
+        <v>50</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <f>1/5 + 0</f>
+        <v>0.2</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23">
+        <v>1500</v>
+      </c>
+      <c r="C23">
+        <v>250</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24">
+        <v>120</v>
+      </c>
+      <c r="C24">
+        <v>25</v>
+      </c>
+      <c r="D24">
+        <f>1/5+1/5</f>
+        <v>0.4</v>
+      </c>
+      <c r="Q24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25">
+        <v>1500</v>
+      </c>
+      <c r="C25">
+        <v>500</v>
+      </c>
+      <c r="Q25">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>